<commit_message>
update lenh dieu xe
</commit_message>
<xml_diff>
--- a/CMS.Web/Modules/Sails/Admin/ExportTemplates/TourCommand.xlsx
+++ b/CMS.Web/Modules/Sails/Admin/ExportTemplates/TourCommand.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\orientalsails\CMS.Web\Modules\Sails\Admin\ExportTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4147591A-28E9-4C5C-A337-7DB368A4D737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F85FBFA-F126-4C77-9D7B-AADB195D5F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -501,9 +501,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -534,68 +531,71 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -940,7 +940,7 @@
   <dimension ref="A1:AB33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+      <selection activeCell="I1" sqref="I1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1407,18 +1407,18 @@
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="79">
+      <c r="E1" s="77">
         <v>40156</v>
       </c>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="80" t="s">
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="80"/>
+      <c r="L1" s="78"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
@@ -1429,8 +1429,8 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="41"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
       <c r="K2" s="2"/>
       <c r="L2" s="4"/>
     </row>
@@ -1446,8 +1446,8 @@
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
       <c r="H3" s="41"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
       <c r="K3" s="2"/>
       <c r="L3" s="4"/>
     </row>
@@ -1463,8 +1463,8 @@
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="H4" s="41"/>
-      <c r="I4" s="56"/>
-      <c r="J4" s="56"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
       <c r="K4" s="2"/>
       <c r="L4" s="4"/>
     </row>
@@ -1480,47 +1480,47 @@
       <c r="E5" s="27"/>
       <c r="F5" s="27"/>
       <c r="H5" s="41"/>
-      <c r="I5" s="57"/>
-      <c r="J5" s="57"/>
+      <c r="I5" s="56"/>
+      <c r="J5" s="56"/>
       <c r="K5" s="2"/>
       <c r="L5" s="31"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A6" s="65" t="s">
+    <row r="6" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="71" t="s">
+      <c r="B6" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="72"/>
-      <c r="D6" s="70" t="s">
+      <c r="C6" s="70"/>
+      <c r="D6" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="70"/>
-      <c r="F6" s="70"/>
-      <c r="G6" s="66" t="s">
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="65" t="s">
+      <c r="H6" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="I6" s="66" t="s">
+      <c r="I6" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="J6" s="61" t="s">
+      <c r="J6" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="K6" s="67" t="s">
+      <c r="K6" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="L6" s="65" t="s">
+      <c r="L6" s="63" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A7" s="65"/>
-      <c r="B7" s="73"/>
-      <c r="C7" s="74"/>
+      <c r="A7" s="63"/>
+      <c r="B7" s="71"/>
+      <c r="C7" s="72"/>
       <c r="D7" s="28" t="s">
         <v>7</v>
       </c>
@@ -1530,17 +1530,17 @@
       <c r="F7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="66"/>
-      <c r="H7" s="65"/>
-      <c r="I7" s="66"/>
-      <c r="J7" s="62"/>
-      <c r="K7" s="68"/>
-      <c r="L7" s="65"/>
+      <c r="G7" s="68"/>
+      <c r="H7" s="63"/>
+      <c r="I7" s="59"/>
+      <c r="J7" s="80"/>
+      <c r="K7" s="65"/>
+      <c r="L7" s="63"/>
     </row>
     <row r="8" spans="1:28" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="24"/>
-      <c r="B8" s="75"/>
-      <c r="C8" s="76"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="74"/>
       <c r="D8" s="24"/>
       <c r="E8" s="24"/>
       <c r="F8" s="24"/>
@@ -1563,8 +1563,8 @@
       <c r="F9" s="29"/>
       <c r="G9" s="16"/>
       <c r="H9" s="43"/>
-      <c r="I9" s="59"/>
-      <c r="J9" s="59"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="58"/>
       <c r="K9" s="16"/>
       <c r="L9" s="16"/>
       <c r="AB9" s="34"/>
@@ -1578,8 +1578,8 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="41"/>
-      <c r="I10" s="56"/>
-      <c r="J10" s="56"/>
+      <c r="I10" s="55"/>
+      <c r="J10" s="55"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
@@ -1594,48 +1594,48 @@
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
       <c r="H11" s="43"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="57"/>
+      <c r="I11" s="56"/>
+      <c r="J11" s="56"/>
       <c r="K11" s="16"/>
       <c r="L11" s="16"/>
       <c r="AB11" s="34"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A12" s="65" t="s">
+    <row r="12" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="71" t="s">
+      <c r="B12" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="72"/>
-      <c r="D12" s="70" t="s">
+      <c r="C12" s="70"/>
+      <c r="D12" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="70"/>
-      <c r="F12" s="70"/>
-      <c r="G12" s="66" t="s">
+      <c r="E12" s="67"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="65" t="s">
+      <c r="H12" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="I12" s="66" t="s">
+      <c r="I12" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="J12" s="61" t="s">
+      <c r="J12" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="K12" s="67" t="s">
+      <c r="K12" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="L12" s="65" t="s">
+      <c r="L12" s="63" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A13" s="65"/>
-      <c r="B13" s="73"/>
-      <c r="C13" s="74"/>
+      <c r="A13" s="63"/>
+      <c r="B13" s="71"/>
+      <c r="C13" s="72"/>
       <c r="D13" s="3" t="s">
         <v>7</v>
       </c>
@@ -1645,17 +1645,17 @@
       <c r="F13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="66"/>
-      <c r="H13" s="65"/>
-      <c r="I13" s="66"/>
-      <c r="J13" s="62"/>
-      <c r="K13" s="68"/>
-      <c r="L13" s="65"/>
+      <c r="G13" s="68"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="59"/>
+      <c r="J13" s="80"/>
+      <c r="K13" s="65"/>
+      <c r="L13" s="63"/>
     </row>
     <row r="14" spans="1:28" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="19"/>
-      <c r="B14" s="77"/>
-      <c r="C14" s="78"/>
+      <c r="B14" s="75"/>
+      <c r="C14" s="76"/>
       <c r="D14" s="19"/>
       <c r="E14" s="19"/>
       <c r="F14" s="19"/>
@@ -1678,8 +1678,8 @@
       <c r="F15" s="29"/>
       <c r="G15" s="16"/>
       <c r="H15" s="43"/>
-      <c r="I15" s="58"/>
-      <c r="J15" s="58"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="57"/>
       <c r="K15" s="16"/>
       <c r="L15" s="16"/>
       <c r="AB15" s="34"/>
@@ -1695,14 +1695,14 @@
       <c r="F16" s="23"/>
       <c r="G16" s="23"/>
       <c r="H16" s="45"/>
-      <c r="I16" s="63" t="s">
+      <c r="I16" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="J16" s="64"/>
-      <c r="K16" s="60" t="s">
+      <c r="J16" s="61"/>
+      <c r="K16" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="L16" s="60"/>
+      <c r="L16" s="62"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
@@ -1717,8 +1717,8 @@
       <c r="F17" s="16"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
-      <c r="I17" s="50"/>
-      <c r="J17" s="51"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="50"/>
       <c r="K17" s="35"/>
       <c r="L17" s="36"/>
     </row>
@@ -1735,8 +1735,8 @@
       <c r="F18" s="16"/>
       <c r="G18" s="1"/>
       <c r="H18" s="46"/>
-      <c r="I18" s="52"/>
-      <c r="J18" s="53"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="52"/>
       <c r="K18" s="37"/>
       <c r="L18" s="38"/>
     </row>
@@ -1749,8 +1749,8 @@
       <c r="F19" s="16"/>
       <c r="G19" s="1"/>
       <c r="H19" s="46"/>
-      <c r="I19" s="52"/>
-      <c r="J19" s="53"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="52"/>
       <c r="K19" s="37"/>
       <c r="L19" s="38"/>
     </row>
@@ -1758,13 +1758,13 @@
       <c r="A20" s="14"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
-      <c r="D20" s="69"/>
-      <c r="E20" s="69"/>
-      <c r="F20" s="69"/>
-      <c r="G20" s="69"/>
+      <c r="D20" s="66"/>
+      <c r="E20" s="66"/>
+      <c r="F20" s="66"/>
+      <c r="G20" s="66"/>
       <c r="H20" s="43"/>
-      <c r="I20" s="54"/>
-      <c r="J20" s="55"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="54"/>
       <c r="K20" s="39"/>
       <c r="L20" s="40"/>
     </row>
@@ -1879,13 +1879,11 @@
       <c r="H33" s="48"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="I6:I7"/>
+  <mergeCells count="22">
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="L6:L7"/>
     <mergeCell ref="K1:L1"/>
-    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="I1:J1"/>
     <mergeCell ref="D20:G20"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A12:A13"/>
@@ -1896,15 +1894,14 @@
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B12:C13"/>
     <mergeCell ref="B14:C14"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="D6:F6"/>
     <mergeCell ref="I16:J16"/>
     <mergeCell ref="K16:L16"/>
     <mergeCell ref="L12:L13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="K12:K13"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>